<commit_message>
changed siteid in loi_data and added to
</commit_message>
<xml_diff>
--- a/loi_data.xlsx
+++ b/loi_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danto\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danto\Documents\00_Work\02_Projects\02_1670_blueCarbon_OCSPN\03_Analyses\AnalyzeBlueCarbon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59B6F83-CAA2-4513-8C99-3DF270B983CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB722E20-3601-4F68-9544-3FB16BC5AB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1260" windowWidth="29040" windowHeight="15840" xr2:uid="{A9BB93D8-0FA2-4C32-A178-B115AFFC29A2}"/>
   </bookViews>
@@ -56,9 +56,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="67">
   <si>
-    <t>SITE-ID</t>
-  </si>
-  <si>
     <t>SECTION</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>CO4 48_49</t>
+  </si>
+  <si>
+    <t>SITEID</t>
   </si>
 </sst>
 </file>
@@ -266,7 +266,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,12 +290,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -556,7 +550,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA429401-B8DA-419C-9628-AA4DCF87B95C}" name="tblMCN" displayName="tblMCN" ref="A1:O51" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A1:O51" xr:uid="{CA429401-B8DA-419C-9628-AA4DCF87B95C}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{9B3A07FE-83C8-40C6-B2AD-79A203C6D341}" name="SITE-ID" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{9B3A07FE-83C8-40C6-B2AD-79A203C6D341}" name="SITEID" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{EE87BDF9-19AA-4123-871F-AA0EBCC82FD9}" name="SECTION" dataDxfId="6"/>
     <tableColumn id="16" xr3:uid="{0F80E074-3CE2-4C45-BDA2-33805881D754}" name="DEPTH_cm" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{FD81C3D0-3BA0-459C-9989-4D2A266F5BCB}" name="δ13C"/>
@@ -910,7 +904,7 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -924,57 +918,57 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="C2" s="6">
         <v>2</v>
@@ -1018,10 +1012,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -1065,10 +1059,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="6">
         <v>2</v>
@@ -1112,10 +1106,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="6">
         <v>2</v>
@@ -1159,10 +1153,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="6">
         <v>2</v>
@@ -1206,10 +1200,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
@@ -1253,10 +1247,10 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="6">
         <v>2</v>
@@ -1300,10 +1294,10 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="6">
         <v>2</v>
@@ -1347,10 +1341,10 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="6">
         <v>2</v>
@@ -1394,10 +1388,10 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="6">
         <v>2</v>
@@ -1441,10 +1435,10 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="6">
         <v>2</v>
@@ -1488,10 +1482,10 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="6">
         <v>2</v>
@@ -1535,10 +1529,10 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="6">
         <v>2</v>
@@ -1582,10 +1576,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="6">
         <v>2</v>
@@ -1629,10 +1623,10 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="6">
         <v>2</v>
@@ -1676,10 +1670,10 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="6">
         <v>2</v>
@@ -1723,10 +1717,10 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="14">
         <v>2</v>
@@ -1772,10 +1766,10 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="6">
         <v>2</v>
@@ -1819,10 +1813,10 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="6">
         <v>2</v>
@@ -1866,10 +1860,10 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="6">
         <v>2</v>
@@ -1913,10 +1907,10 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="6">
         <v>2</v>
@@ -1960,10 +1954,10 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="6">
         <v>2</v>
@@ -2007,10 +2001,10 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="6">
         <v>2</v>
@@ -2054,10 +2048,10 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="6">
         <v>2</v>
@@ -2101,10 +2095,10 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="6">
         <v>2</v>
@@ -2148,10 +2142,10 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="C27" s="6">
         <v>2</v>
@@ -2195,10 +2189,10 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="6">
         <v>2</v>
@@ -2242,10 +2236,10 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C29" s="6">
         <v>2</v>
@@ -2289,10 +2283,10 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" s="6">
         <v>2</v>
@@ -2336,10 +2330,10 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" s="6">
         <v>2</v>
@@ -2383,10 +2377,10 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="6">
         <v>2</v>
@@ -2430,10 +2424,10 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="6">
         <v>2</v>
@@ -2477,10 +2471,10 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" s="6">
         <v>2</v>
@@ -2524,10 +2518,10 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" s="14">
         <v>2</v>
@@ -2573,10 +2567,10 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="14">
         <v>2</v>
@@ -2622,10 +2616,10 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="14">
         <v>2</v>
@@ -2671,10 +2665,10 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38" s="14">
         <v>2</v>
@@ -2720,10 +2714,10 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39" s="14">
         <v>2</v>
@@ -2769,10 +2763,10 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C40" s="6">
         <v>2</v>
@@ -2816,10 +2810,10 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" s="14">
         <v>2</v>
@@ -2865,10 +2859,10 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C42" s="14">
         <v>2</v>
@@ -2914,10 +2908,10 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C43" s="14">
         <v>2</v>
@@ -2963,10 +2957,10 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C44" s="14">
         <v>2</v>
@@ -3012,10 +3006,10 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" s="14">
         <v>2</v>
@@ -3061,10 +3055,10 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" s="14">
         <v>2</v>
@@ -3110,10 +3104,10 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="6">
         <v>2</v>
@@ -3157,10 +3151,10 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48" s="6">
         <v>2</v>
@@ -3204,10 +3198,10 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" s="6">
         <v>2</v>
@@ -3251,10 +3245,10 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C50" s="6">
         <v>2</v>
@@ -3298,10 +3292,10 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C51" s="14">
         <v>2</v>

</xml_diff>